<commit_message>
midst of editing welfare_analysis_framework
about to move NC_no_human code into visualisations. Spent this time making sure NC and WR are always run togeter, reorganising the way results end up in directories, etc.

Have also created wild_animal_module, on the way to including wild animal outputs.
</commit_message>
<xml_diff>
--- a/first_pass/welfare_results/isoelastic_WR/human_data_formatted.xlsx
+++ b/first_pass/welfare_results/isoelastic_WR/human_data_formatted.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">NC_potential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forebrain_neurons</t>
   </si>
   <si>
     <t xml:space="preserve">Humans</t>
@@ -389,16 +392,19 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1960</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
         <v>3010827523</v>
@@ -411,6 +417,9 @@
       </c>
       <c r="G2" t="n">
         <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="3">
@@ -418,10 +427,10 @@
         <v>1961</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>3051697141</v>
@@ -434,6 +443,9 @@
       </c>
       <c r="G3" t="n">
         <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +453,10 @@
         <v>1962</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v>3105920620</v>
@@ -457,6 +469,9 @@
       </c>
       <c r="G4" t="n">
         <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="5">
@@ -464,10 +479,10 @@
         <v>1963</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
         <v>3172220909</v>
@@ -480,6 +495,9 @@
       </c>
       <c r="G5" t="n">
         <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="6">
@@ -487,10 +505,10 @@
         <v>1964</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
         <v>3239011665</v>
@@ -503,6 +521,9 @@
       </c>
       <c r="G6" t="n">
         <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="7">
@@ -510,10 +531,10 @@
         <v>1965</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
         <v>3306347796</v>
@@ -526,6 +547,9 @@
       </c>
       <c r="G7" t="n">
         <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="8">
@@ -533,10 +557,10 @@
         <v>1966</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
         <v>3376019383</v>
@@ -549,6 +573,9 @@
       </c>
       <c r="G8" t="n">
         <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="9">
@@ -556,10 +583,10 @@
         <v>1967</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="n">
         <v>3445805012</v>
@@ -572,6 +599,9 @@
       </c>
       <c r="G9" t="n">
         <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="10">
@@ -579,10 +609,10 @@
         <v>1968</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
         <v>3517155024</v>
@@ -595,6 +625,9 @@
       </c>
       <c r="G10" t="n">
         <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="11">
@@ -602,10 +635,10 @@
         <v>1969</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
         <v>3590757761</v>
@@ -618,6 +651,9 @@
       </c>
       <c r="G11" t="n">
         <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="12">
@@ -625,10 +661,10 @@
         <v>1970</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" t="n">
         <v>3666017294</v>
@@ -641,6 +677,9 @@
       </c>
       <c r="G12" t="n">
         <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="13">
@@ -648,10 +687,10 @@
         <v>1971</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
         <v>3743699982</v>
@@ -664,6 +703,9 @@
       </c>
       <c r="G13" t="n">
         <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="14">
@@ -671,10 +713,10 @@
         <v>1972</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="n">
         <v>3819225827</v>
@@ -687,6 +729,9 @@
       </c>
       <c r="G14" t="n">
         <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="15">
@@ -694,10 +739,10 @@
         <v>1973</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" t="n">
         <v>3895563337</v>
@@ -710,6 +755,9 @@
       </c>
       <c r="G15" t="n">
         <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="16">
@@ -717,10 +765,10 @@
         <v>1974</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" t="n">
         <v>3971509423</v>
@@ -733,6 +781,9 @@
       </c>
       <c r="G16" t="n">
         <v>1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="17">
@@ -740,10 +791,10 @@
         <v>1975</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
         <v>4045995643</v>
@@ -756,6 +807,9 @@
       </c>
       <c r="G17" t="n">
         <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="18">
@@ -763,10 +817,10 @@
         <v>1976</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
         <v>4119357126</v>
@@ -779,6 +833,9 @@
       </c>
       <c r="G18" t="n">
         <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="19">
@@ -786,10 +843,10 @@
         <v>1977</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="n">
         <v>4192227909</v>
@@ -802,6 +859,9 @@
       </c>
       <c r="G19" t="n">
         <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="20">
@@ -809,10 +869,10 @@
         <v>1978</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" t="n">
         <v>4266388771</v>
@@ -825,6 +885,9 @@
       </c>
       <c r="G20" t="n">
         <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="21">
@@ -832,10 +895,10 @@
         <v>1979</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D21" t="n">
         <v>4342683622</v>
@@ -848,6 +911,9 @@
       </c>
       <c r="G21" t="n">
         <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="22">
@@ -855,10 +921,10 @@
         <v>1980</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="n">
         <v>4419898354</v>
@@ -871,6 +937,9 @@
       </c>
       <c r="G22" t="n">
         <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="23">
@@ -878,10 +947,10 @@
         <v>1981</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
         <v>4498896208</v>
@@ -894,6 +963,9 @@
       </c>
       <c r="G23" t="n">
         <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="24">
@@ -901,10 +973,10 @@
         <v>1982</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" t="n">
         <v>4581184386</v>
@@ -917,6 +989,9 @@
       </c>
       <c r="G24" t="n">
         <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="25">
@@ -924,10 +999,10 @@
         <v>1983</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" t="n">
         <v>4664271390</v>
@@ -940,6 +1015,9 @@
       </c>
       <c r="G25" t="n">
         <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="26">
@@ -947,10 +1025,10 @@
         <v>1984</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" t="n">
         <v>4747110434</v>
@@ -963,6 +1041,9 @@
       </c>
       <c r="G26" t="n">
         <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="27">
@@ -970,10 +1051,10 @@
         <v>1985</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" t="n">
         <v>4831549278</v>
@@ -986,6 +1067,9 @@
       </c>
       <c r="G27" t="n">
         <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="28">
@@ -993,10 +1077,10 @@
         <v>1986</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
         <v>4918300108</v>
@@ -1009,6 +1093,9 @@
       </c>
       <c r="G28" t="n">
         <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="29">
@@ -1016,10 +1103,10 @@
         <v>1987</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" t="n">
         <v>5007413232</v>
@@ -1032,6 +1119,9 @@
       </c>
       <c r="G29" t="n">
         <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="30">
@@ -1039,10 +1129,10 @@
         <v>1988</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D30" t="n">
         <v>5097327302</v>
@@ -1055,6 +1145,9 @@
       </c>
       <c r="G30" t="n">
         <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="31">
@@ -1062,10 +1155,10 @@
         <v>1989</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31" t="n">
         <v>5187599374</v>
@@ -1078,6 +1171,9 @@
       </c>
       <c r="G31" t="n">
         <v>1</v>
+      </c>
+      <c r="H31" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="32">
@@ -1085,10 +1181,10 @@
         <v>1990</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n">
         <v>5278967811</v>
@@ -1101,6 +1197,9 @@
       </c>
       <c r="G32" t="n">
         <v>1</v>
+      </c>
+      <c r="H32" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="33">
@@ -1108,10 +1207,10 @@
         <v>1991</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n">
         <v>5367992660</v>
@@ -1124,6 +1223,9 @@
       </c>
       <c r="G33" t="n">
         <v>1</v>
+      </c>
+      <c r="H33" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="34">
@@ -1131,10 +1233,10 @@
         <v>1992</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34" t="n">
         <v>5456438624.5</v>
@@ -1147,6 +1249,9 @@
       </c>
       <c r="G34" t="n">
         <v>1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="35">
@@ -1154,10 +1259,10 @@
         <v>1993</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" t="n">
         <v>5543904800</v>
@@ -1170,6 +1275,9 @@
       </c>
       <c r="G35" t="n">
         <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="36">
@@ -1177,10 +1285,10 @@
         <v>1994</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" t="n">
         <v>5629775894.5</v>
@@ -1193,6 +1301,9 @@
       </c>
       <c r="G36" t="n">
         <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="37">
@@ -1200,10 +1311,10 @@
         <v>1995</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D37" t="n">
         <v>5715247477</v>
@@ -1216,6 +1327,9 @@
       </c>
       <c r="G37" t="n">
         <v>1</v>
+      </c>
+      <c r="H37" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="38">
@@ -1223,10 +1337,10 @@
         <v>1996</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D38" t="n">
         <v>5801190546.5</v>
@@ -1239,6 +1353,9 @@
       </c>
       <c r="G38" t="n">
         <v>1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="39">
@@ -1246,10 +1363,10 @@
         <v>1997</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" t="n">
         <v>5886866405.5</v>
@@ -1262,6 +1379,9 @@
       </c>
       <c r="G39" t="n">
         <v>1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="40">
@@ -1269,10 +1389,10 @@
         <v>1998</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40" t="n">
         <v>5972206291.5</v>
@@ -1285,6 +1405,9 @@
       </c>
       <c r="G40" t="n">
         <v>1</v>
+      </c>
+      <c r="H40" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="41">
@@ -1292,10 +1415,10 @@
         <v>1999</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" t="n">
         <v>6056396446</v>
@@ -1308,6 +1431,9 @@
       </c>
       <c r="G41" t="n">
         <v>1</v>
+      </c>
+      <c r="H41" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="42">
@@ -1315,10 +1441,10 @@
         <v>2000</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" t="n">
         <v>6139712296.5</v>
@@ -1331,6 +1457,9 @@
       </c>
       <c r="G42" t="n">
         <v>1</v>
+      </c>
+      <c r="H42" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="43">
@@ -1338,10 +1467,10 @@
         <v>2001</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" t="n">
         <v>6222770459.5</v>
@@ -1354,6 +1483,9 @@
       </c>
       <c r="G43" t="n">
         <v>1</v>
+      </c>
+      <c r="H43" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="44">
@@ -1361,10 +1493,10 @@
         <v>2002</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" t="n">
         <v>6305069108</v>
@@ -1377,6 +1509,9 @@
       </c>
       <c r="G44" t="n">
         <v>1</v>
+      </c>
+      <c r="H44" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="45">
@@ -1384,10 +1519,10 @@
         <v>2003</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D45" t="n">
         <v>6387110221</v>
@@ -1400,6 +1535,9 @@
       </c>
       <c r="G45" t="n">
         <v>1</v>
+      </c>
+      <c r="H45" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="46">
@@ -1407,10 +1545,10 @@
         <v>2004</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D46" t="n">
         <v>6469986725.5</v>
@@ -1423,6 +1561,9 @@
       </c>
       <c r="G46" t="n">
         <v>1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="47">
@@ -1430,10 +1571,10 @@
         <v>2005</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47" t="n">
         <v>6552921748.5</v>
@@ -1446,6 +1587,9 @@
       </c>
       <c r="G47" t="n">
         <v>1</v>
+      </c>
+      <c r="H47" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="48">
@@ -1453,10 +1597,10 @@
         <v>2006</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D48" t="n">
         <v>6636906506</v>
@@ -1469,6 +1613,9 @@
       </c>
       <c r="G48" t="n">
         <v>1</v>
+      </c>
+      <c r="H48" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="49">
@@ -1476,10 +1623,10 @@
         <v>2007</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D49" t="n">
         <v>6721269564.5</v>
@@ -1492,6 +1639,9 @@
       </c>
       <c r="G49" t="n">
         <v>1</v>
+      </c>
+      <c r="H49" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="50">
@@ -1499,10 +1649,10 @@
         <v>2008</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50" t="n">
         <v>6807134829</v>
@@ -1515,6 +1665,9 @@
       </c>
       <c r="G50" t="n">
         <v>1</v>
+      </c>
+      <c r="H50" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="51">
@@ -1522,10 +1675,10 @@
         <v>2009</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D51" t="n">
         <v>6893059682</v>
@@ -1538,6 +1691,9 @@
       </c>
       <c r="G51" t="n">
         <v>1</v>
+      </c>
+      <c r="H51" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="52">
@@ -1545,10 +1701,10 @@
         <v>2010</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D52" t="n">
         <v>6977532852</v>
@@ -1561,6 +1717,9 @@
       </c>
       <c r="G52" t="n">
         <v>1</v>
+      </c>
+      <c r="H52" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="53">
@@ -1568,10 +1727,10 @@
         <v>2011</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D53" t="n">
         <v>7063021186.5</v>
@@ -1584,6 +1743,9 @@
       </c>
       <c r="G53" t="n">
         <v>1</v>
+      </c>
+      <c r="H53" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="54">
@@ -1591,10 +1753,10 @@
         <v>2012</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D54" t="n">
         <v>7152554638</v>
@@ -1607,6 +1769,9 @@
       </c>
       <c r="G54" t="n">
         <v>1</v>
+      </c>
+      <c r="H54" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="55">
@@ -1614,10 +1779,10 @@
         <v>2013</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D55" t="n">
         <v>7241970754</v>
@@ -1630,6 +1795,9 @@
       </c>
       <c r="G55" t="n">
         <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="56">
@@ -1637,10 +1805,10 @@
         <v>2014</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56" t="n">
         <v>7330518889.5</v>
@@ -1653,6 +1821,9 @@
       </c>
       <c r="G56" t="n">
         <v>1</v>
+      </c>
+      <c r="H56" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="57">
@@ -1660,10 +1831,10 @@
         <v>2015</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D57" t="n">
         <v>7418010158.5</v>
@@ -1676,6 +1847,9 @@
       </c>
       <c r="G57" t="n">
         <v>1</v>
+      </c>
+      <c r="H57" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="58">
@@ -1683,10 +1857,10 @@
         <v>2016</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D58" t="n">
         <v>7505014971.5</v>
@@ -1699,6 +1873,9 @@
       </c>
       <c r="G58" t="n">
         <v>1</v>
+      </c>
+      <c r="H58" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="59">
@@ -1706,10 +1883,10 @@
         <v>2017</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59" t="n">
         <v>7590561081.5</v>
@@ -1722,6 +1899,9 @@
       </c>
       <c r="G59" t="n">
         <v>1</v>
+      </c>
+      <c r="H59" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="60">
@@ -1729,10 +1909,10 @@
         <v>2018</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D60" t="n">
         <v>7672920573.5</v>
@@ -1745,6 +1925,9 @@
       </c>
       <c r="G60" t="n">
         <v>1</v>
+      </c>
+      <c r="H60" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="61">
@@ -1752,10 +1935,10 @@
         <v>2019</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D61" t="n">
         <v>7753300984</v>
@@ -1768,6 +1951,9 @@
       </c>
       <c r="G61" t="n">
         <v>1</v>
+      </c>
+      <c r="H61" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="62">
@@ -1775,10 +1961,10 @@
         <v>2020</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D62" t="n">
         <v>7832554966.5</v>
@@ -1791,6 +1977,9 @@
       </c>
       <c r="G62" t="n">
         <v>1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="63">
@@ -1798,10 +1987,10 @@
         <v>2021</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
         <v>7897696837</v>
@@ -1814,6 +2003,9 @@
       </c>
       <c r="G63" t="n">
         <v>1</v>
+      </c>
+      <c r="H63" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="64">
@@ -1821,10 +2013,10 @@
         <v>2022</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D64" t="n">
         <v>7966795241.5</v>
@@ -1837,6 +2029,9 @@
       </c>
       <c r="G64" t="n">
         <v>1</v>
+      </c>
+      <c r="H64" t="n">
+        <v>24560000000</v>
       </c>
     </row>
     <row r="65">
@@ -1844,10 +2039,10 @@
         <v>2023</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D65" t="n">
         <v>8038502718</v>
@@ -1860,6 +2055,9 @@
       </c>
       <c r="G65" t="n">
         <v>1</v>
+      </c>
+      <c r="H65" t="n">
+        <v>24560000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>